<commit_message>
Removendo Coluna Duplicada Product Backlog
</commit_message>
<xml_diff>
--- a/Sprint 3/Planejamento/Backlog - Final.xlsx
+++ b/Sprint 3/Planejamento/Backlog - Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hiago Farias\Desktop\PROJETO - SENTINELA\Grupo-3\Sprint 3\Planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED677D92-8279-4B56-84BE-20D1C612790A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EFD12F-B2A6-41F0-8C74-FDFDC4914F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="304" xr2:uid="{01FB4863-7F38-4DC3-AD03-162B05A03864}"/>
   </bookViews>
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E490A3FA-AB2E-4D68-B0D5-05FAAD73C7D1}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:H45"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2973,7 +2973,7 @@
         <v>90</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>69</v>
@@ -3373,14 +3373,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1dc861b8-2196-455d-b291-a999da8cffb6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045B33021656A9E479DF12B9A8EE42828" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1f4cc90d25b18fe9fc6767603d58113">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1dc861b8-2196-455d-b291-a999da8cffb6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19f91625984506300aae7074362d9652" ns3:_="">
     <xsd:import namespace="1dc861b8-2196-455d-b291-a999da8cffb6"/>
@@ -3536,6 +3528,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1dc861b8-2196-455d-b291-a999da8cffb6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3546,22 +3546,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{367DAA4C-4F4B-4445-A313-DAF4BECB4137}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1dc861b8-2196-455d-b291-a999da8cffb6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB07C1AA-5987-4ED4-B5B1-BDA6B66B83A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3580,6 +3564,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{367DAA4C-4F4B-4445-A313-DAF4BECB4137}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1dc861b8-2196-455d-b291-a999da8cffb6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA97BAC9-A765-458E-B3E5-66999EAB8036}">
   <ds:schemaRefs>

</xml_diff>